<commit_message>
- add STAGE_MAP to ASSUMPTIONS.xlsx - add basic CLI - rename 'stage' in account level data to 'watchlist' so that it is not confused with the stage produced by the model
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbisschoff\Desktop\Playground\Z-model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A402BAB-A70F-4ECF-B937-242EF51E1671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
     <sheet name="TRANSITION_MATRIX" sheetId="3" r:id="rId2"/>
-    <sheet name="DICTIONARY" sheetId="4" r:id="rId3"/>
+    <sheet name="STAGE_MAP" sheetId="5" r:id="rId3"/>
+    <sheet name="DICTIONARY" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TRANSITION_MATRIX!$A$1:$A$29</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>segment_name</t>
   </si>
@@ -247,11 +249,17 @@
 - METHOD 2: EAD = limit * CCF
 - METHOD 3: EAD = outstanding_balance + (limit - outstanding_balance) * CCF</t>
   </si>
+  <si>
+    <t>origination/current</t>
+  </si>
+  <si>
+    <t>WO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -306,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -409,11 +417,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -474,11 +493,82 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -753,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection sqref="A1:X1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,10 +1191,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1599,13 +1689,181 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A29"/>
+  <autoFilter ref="A1:A29" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B0E0E0-37B0-4251-B8B8-6CCA50F4DCCD}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="30">
+        <v>0</v>
+      </c>
+      <c r="C1" s="30">
+        <v>1</v>
+      </c>
+      <c r="D1" s="30">
+        <v>2</v>
+      </c>
+      <c r="E1" s="30">
+        <v>3</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>0</v>
+      </c>
+      <c r="B2" s="32">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33">
+        <v>1</v>
+      </c>
+      <c r="D2" s="33">
+        <v>2</v>
+      </c>
+      <c r="E2" s="33">
+        <v>2</v>
+      </c>
+      <c r="F2" s="33">
+        <v>3</v>
+      </c>
+      <c r="G2" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <v>1</v>
+      </c>
+      <c r="B3" s="35">
+        <v>1</v>
+      </c>
+      <c r="C3" s="36">
+        <v>1</v>
+      </c>
+      <c r="D3" s="36">
+        <v>2</v>
+      </c>
+      <c r="E3" s="36">
+        <v>2</v>
+      </c>
+      <c r="F3" s="36">
+        <v>3</v>
+      </c>
+      <c r="G3" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="35">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36">
+        <v>1</v>
+      </c>
+      <c r="D4" s="36">
+        <v>1</v>
+      </c>
+      <c r="E4" s="36">
+        <v>2</v>
+      </c>
+      <c r="F4" s="36">
+        <v>3</v>
+      </c>
+      <c r="G4" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>3</v>
+      </c>
+      <c r="B5" s="35">
+        <v>1</v>
+      </c>
+      <c r="C5" s="36">
+        <v>1</v>
+      </c>
+      <c r="D5" s="36">
+        <v>1</v>
+      </c>
+      <c r="E5" s="36">
+        <v>2</v>
+      </c>
+      <c r="F5" s="36">
+        <v>3</v>
+      </c>
+      <c r="G5" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="38">
+        <v>3</v>
+      </c>
+      <c r="C6" s="39">
+        <v>3</v>
+      </c>
+      <c r="D6" s="39">
+        <v>3</v>
+      </c>
+      <c r="E6" s="39">
+        <v>3</v>
+      </c>
+      <c r="F6" s="39">
+        <v>3</v>
+      </c>
+      <c r="G6" s="40">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:G6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
Change  the way the model executes. In the prior version it was at an account level, i.e. each account had an ECLModel() class, now the model is executed at a segment level, i.e. each segment has a ECLModel() class.
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A402BAB-A70F-4ECF-B937-242EF51E1671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F9B194-A75D-411B-BF7E-B6E4914901D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
   <si>
     <t>segment_name</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>pd_z_index</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
   <si>
     <t>Field</t>
@@ -254,6 +251,15 @@
   </si>
   <si>
     <t>WO</t>
+  </si>
+  <si>
+    <t>pd_redemption_freq</t>
+  </si>
+  <si>
+    <t>ead_fees_fixed</t>
+  </si>
+  <si>
+    <t>lgd_sale_cost</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -526,25 +532,19 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -560,11 +560,18 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -844,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,27 +865,28 @@
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -898,61 +906,64 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="V1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -971,50 +982,53 @@
       <c r="F2" s="5">
         <v>0.05</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="41">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="5">
         <v>0.15</v>
       </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
       <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
         <v>0.25</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="5">
         <v>0.05</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>12</v>
       </c>
-      <c r="P2" s="5">
+      <c r="Q2" s="5">
         <v>0.01</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-      <c r="U2" s="2">
+      <c r="U2" s="5"/>
+      <c r="V2" s="2">
         <v>0.5</v>
-      </c>
-      <c r="V2" s="3">
-        <v>1E-3</v>
       </c>
       <c r="W2" s="3">
         <v>1E-3</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1033,50 +1047,53 @@
       <c r="F3" s="5">
         <v>0.05</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="41">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>0.3</v>
       </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
       <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
         <v>0.25</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N3" s="5">
         <v>0.05</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>12</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="5">
         <v>0.01</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="2">
+      <c r="U3" s="5"/>
+      <c r="V3" s="2">
         <v>0.5</v>
-      </c>
-      <c r="V3" s="3">
-        <v>1E-3</v>
       </c>
       <c r="W3" s="3">
         <v>1E-3</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X3" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1095,42 +1112,45 @@
       <c r="F4" s="5">
         <v>0.05</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="41">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="J4" s="6">
+      <c r="I4" s="2"/>
+      <c r="K4" s="6">
         <v>0.5</v>
       </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
         <v>12</v>
       </c>
-      <c r="O4" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="2">
+      <c r="U4" s="5"/>
+      <c r="V4" s="2">
         <v>0.5</v>
-      </c>
-      <c r="V4" s="3">
-        <v>1E-3</v>
       </c>
       <c r="W4" s="3">
         <v>1E-3</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="X4" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1149,38 +1169,41 @@
       <c r="F5" s="5">
         <v>0.05</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="41">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="I5" s="2"/>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
         <v>12</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <v>0.7</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="2">
+      <c r="U5" s="5"/>
+      <c r="V5" s="2">
         <v>0.5</v>
-      </c>
-      <c r="V5" s="3">
-        <v>1E-3</v>
       </c>
       <c r="W5" s="3">
         <v>1E-3</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="X5" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="Y5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1195,7 +1218,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,8 +1247,8 @@
       <c r="F1" s="1">
         <v>3</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>37</v>
+      <c r="G1" s="9">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1324,8 +1347,8 @@
       <c r="A6" s="27">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>37</v>
+      <c r="B6" s="28">
+        <v>4</v>
       </c>
       <c r="C6" s="22">
         <v>0</v>
@@ -1439,8 +1462,8 @@
       <c r="A11" s="27">
         <v>2</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>37</v>
+      <c r="B11" s="28">
+        <v>4</v>
       </c>
       <c r="C11" s="22">
         <v>0</v>
@@ -1554,8 +1577,8 @@
       <c r="A16" s="27">
         <v>3</v>
       </c>
-      <c r="B16" s="28" t="s">
-        <v>37</v>
+      <c r="B16" s="28">
+        <v>4</v>
       </c>
       <c r="C16" s="22">
         <v>0</v>
@@ -1669,8 +1692,8 @@
       <c r="A21" s="27">
         <v>4</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>37</v>
+      <c r="B21" s="28">
+        <v>4</v>
       </c>
       <c r="C21" s="22">
         <v>0</v>
@@ -1691,6 +1714,7 @@
   </sheetData>
   <autoFilter ref="A1:A29" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1699,14 +1723,17 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="30">
         <v>0</v>
@@ -1720,11 +1747,11 @@
       <c r="E1" s="30">
         <v>3</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>37</v>
+      <c r="F1" s="30">
+        <v>4</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1820,8 +1847,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
-        <v>37</v>
+      <c r="A6" s="31">
+        <v>4</v>
       </c>
       <c r="B6" s="38">
         <v>3</v>
@@ -1844,16 +1871,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:G6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1879,13 +1906,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,10 +1920,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1904,10 +1931,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1915,10 +1942,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,10 +1953,10 @@
         <v>36</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1937,10 +1964,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,10 +1975,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1959,10 +1986,10 @@
         <v>27</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,10 +1997,10 @@
         <v>32</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,10 +2008,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,10 +2019,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,10 +2030,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,10 +2041,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,10 +2052,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2036,10 +2063,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2047,10 +2074,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,10 +2085,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2069,10 +2096,10 @@
         <v>30</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,10 +2107,10 @@
         <v>33</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -2091,10 +2118,10 @@
         <v>34</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2102,10 +2129,10 @@
         <v>35</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2113,10 +2140,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2124,10 +2151,10 @@
         <v>14</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2135,10 +2162,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2146,10 +2173,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update readme and example assumptions file.
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDA3801-3B84-45EA-83E7-290C1691FCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9508D412-1A12-42CD-9514-CC3700ACABB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40452" yWindow="-6528" windowWidth="40560" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40452" yWindow="-6528" windowWidth="40560" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
   <si>
     <t>segment_name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>pd_rho</t>
   </si>
   <si>
-    <t>pd_redemption_rate</t>
-  </si>
-  <si>
     <t>lgd_probability_of_cure</t>
   </si>
   <si>
@@ -173,16 +170,10 @@
     <t>&lt;int&gt;</t>
   </si>
   <si>
-    <t>The type of PD model to run. Only TRANSITION_MATRIX is currently supported.</t>
-  </si>
-  <si>
     <t>The Z-index to look up from the Scenarios.</t>
   </si>
   <si>
     <t>The asset correlation parameter Rho.</t>
-  </si>
-  <si>
-    <t>The monthlty redemption rate / closed good used in the survival model.</t>
   </si>
   <si>
     <t>The LGD model to apply. The following values are supported:
@@ -290,6 +281,39 @@
   <si>
     <t>lgd_mu_w</t>
   </si>
+  <si>
+    <t>&lt;bool&gt;</t>
+  </si>
+  <si>
+    <t>Use two diffetent Merton Vasicek formulas:
+If False: 
+    Use the standard MV formula 
+    PiT = N((TtC -  Z * Rho ** 0.5) / (1 - Rho) ** 0.5)
+If True:
+    Add a calibration factor (d) to Z so that the PiT PD = TtC PD if Z=0.
+    PiT = N((TtC -  (Z + d) * Rho ** 0.5) / (1 - Rho) ** 0.5)
+    It can be shown that the formula simplifies to:
+    PiT = N(TtC -  Z * (Rho ** 0.5) / (1 - Rho) ** 0.5)</t>
+  </si>
+  <si>
+    <t>The default state column index in the Transition Matrix</t>
+  </si>
+  <si>
+    <t>The frequency of the transition matrix</t>
+  </si>
+  <si>
+    <t>The number of months an account should remain in the watchlist. This is used for stress testing, does not affect IFRS9 numbers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of PD model to run. Only TRANSITION_MATRIX is currently supported.
+The transition matrix supports both single and multiple default definitions. </t>
+  </si>
+  <si>
+    <t>Calculated field. The resiprocal of the average time to cure. Calculated from the PCURE and TTS assumptions.</t>
+  </si>
+  <si>
+    <t>Calculated field. The resiprocal of the average time to sale. Calculated from the TTS assumptions.</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +322,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -459,7 +483,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -571,9 +595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>565785</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -591,7 +615,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7566660" y="232410"/>
-              <a:ext cx="5189220" cy="2358390"/>
+              <a:ext cx="5191125" cy="2678430"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -625,6 +649,28 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>To calculate the probability of cure and write-off over t</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="1" baseline="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> periods from the time to sale and the lifetime probability of cure assumptions:</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:endParaRPr lang="en-GB" sz="1100" b="0" i="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -685,7 +731,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -698,7 +744,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -712,7 +758,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -726,7 +772,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -738,7 +784,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -750,7 +796,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -867,6 +913,7 @@
               <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -983,7 +1030,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1010,7 +1057,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1026,7 +1073,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1040,7 +1087,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1052,7 +1099,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1070,7 +1117,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1083,7 +1130,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1097,7 +1144,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1126,7 +1173,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1138,7 +1185,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1170,7 +1217,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1183,7 +1230,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1197,7 +1244,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1213,7 +1260,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1227,7 +1274,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1239,7 +1286,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1257,7 +1304,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1270,7 +1317,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1284,7 +1331,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1300,7 +1347,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1313,7 +1360,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1325,7 +1372,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1346,6 +1393,7 @@
               <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1682,6 +1730,7 @@
               <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1843,7 +1892,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1856,7 +1905,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1873,7 +1922,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1886,7 +1935,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1904,7 +1953,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1917,7 +1966,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1929,7 +1978,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1962,7 +2011,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7566660" y="232410"/>
-              <a:ext cx="5189220" cy="2358390"/>
+              <a:ext cx="5191125" cy="2678430"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1996,11 +2045,33 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>To calculate the probability of cure and write-off over t</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="1" baseline="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> periods from the time to sale and the lifetime probability of cure assumptions:</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:endParaRPr lang="en-GB" sz="1100" b="0" i="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>lim_(𝑡</a:t>
+                <a:t>lim┬(𝑡</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -2015,23 +2086,11 @@
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑃_𝐷𝐶 (0,𝑡)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>〗</a:t>
+                <a:t>𝑃_𝐷𝐶 (0,𝑡)〗</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -2045,6 +2104,7 @@
               <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2057,119 +2117,11 @@
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>(1−</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>lim┬(𝑡→∞)〗⁡〖𝑃_𝐷𝐶</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> (</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0,𝑡</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>〗</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>))/</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>〖1−lim┬(𝑡→∞)〗⁡〖𝑃_𝐷𝐶 (0,𝑡)〗</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> </a:t>
+                <a:t>〖(1−lim┬(𝑡→∞)〗⁡〖𝑃_𝐷𝐶 (0,𝑡)〗))/〖1−lim┬(𝑡→∞)〗⁡〖𝑃_𝐷𝐶 (0,𝑡)〗 </a:t>
               </a:r>
               <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
             </a:p>
@@ -2177,11 +2129,12 @@
               <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑃_(𝐷𝐷) ̅  (0,𝑡)=exp⁡(−∫24_0^𝑡▒〖𝜇_𝑐+𝜇_𝑤 〗  𝑑𝑡)=exp⁡(−𝑡(𝜇_𝑐+𝜇_𝑤 ))</a:t>
+                <a:t>𝑃_(𝐷𝐷) ̅  (0,𝑡)=exp⁡(−∫_0^𝑡▒〖𝜇_𝑐+𝜇_𝑤 〗  𝑑𝑡)=exp⁡(−𝑡(𝜇_𝑐+𝜇_𝑤 ))</a:t>
               </a:r>
               <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
@@ -2189,6 +2142,7 @@
               <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2201,23 +2155,11 @@
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑃_(𝐷𝐷) ̅  (0,𝑡)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>)</a:t>
+                <a:t>𝑃_(𝐷𝐷) ̅  (0,𝑡))</a:t>
               </a:r>
               <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
@@ -2495,9 +2437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2539,99 +2479,99 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3">
         <v>0.15540000000000001</v>
@@ -2649,10 +2589,10 @@
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5">
         <v>0.15</v>
@@ -2681,7 +2621,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
@@ -2696,21 +2636,21 @@
         <v>1E-3</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3">
         <v>0.14680000000000001</v>
@@ -2728,10 +2668,10 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="5">
         <v>0.3</v>
@@ -2760,7 +2700,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
@@ -2775,21 +2715,21 @@
         <v>1E-3</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4">
         <v>0.1153</v>
@@ -2807,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="2"/>
       <c r="M4" s="6">
@@ -2831,7 +2771,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
@@ -2846,21 +2786,21 @@
         <v>1E-3</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4">
         <v>0.10680000000000001</v>
@@ -2878,7 +2818,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="2"/>
       <c r="M5" s="6">
@@ -2902,7 +2842,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -2917,7 +2857,7 @@
         <v>1E-3</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2930,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,10 +2893,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D1" s="17">
         <v>1</v>
@@ -2971,10 +2911,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2982,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="24">
         <v>1</v>
@@ -3127,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="15">
         <v>0</v>
@@ -3159,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="28">
         <v>0</v>
@@ -3188,7 +3128,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="24">
         <v>1</v>
@@ -3333,7 +3273,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" s="15">
         <v>0</v>
@@ -3365,7 +3305,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C15" s="28">
         <v>0</v>
@@ -3394,7 +3334,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C16" s="24">
         <v>1</v>
@@ -3539,7 +3479,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C21" s="15">
         <v>0</v>
@@ -3571,7 +3511,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" s="28">
         <v>0</v>
@@ -3600,7 +3540,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C23" s="24">
         <v>1</v>
@@ -3745,7 +3685,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" s="15">
         <v>0</v>
@@ -3777,7 +3717,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C29" s="28">
         <v>0</v>
@@ -3825,10 +3765,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C1" s="17">
         <v>1</v>
@@ -3843,10 +3783,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3992,10 +3932,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4007,13 +3947,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4021,10 +3961,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4032,32 +3972,32 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4065,219 +4005,274 @@
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="13" t="s">
+      <c r="C28" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="13" t="s">
+      <c r="C29" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>41</v>
+      <c r="C30" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add two Z-TM methods. The first uses the Z-risk engine methodology (variable bin widths), the second the Credit Metrics method (fixed bin widths)
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9508D412-1A12-42CD-9514-CC3700ACABB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1761419D-063F-4F0D-BB6E-2998D6556D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40452" yWindow="-6528" windowWidth="40560" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37920" yWindow="-4236" windowWidth="30084" windowHeight="12708" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
   <si>
     <t>segment_name</t>
   </si>
@@ -313,6 +313,20 @@
   </si>
   <si>
     <t>Calculated field. The resiprocal of the average time to sale. Calculated from the TTS assumptions.</t>
+  </si>
+  <si>
+    <t>pd_method</t>
+  </si>
+  <si>
+    <t>METHOD-1</t>
+  </si>
+  <si>
+    <t>The Z-model method to use to calculate the FiT TM.
+METHOD-1: 
+    Use the Z-risk engine method where bin widths are also transformed via the Z-factor.
+    Typically leads to more macro sensitivity and higher PDs.
+METHOD-2:
+    Use the Credit Metrics method where bin widths are fixed and only shifted by the Z-factor.</t>
   </si>
 </sst>
 </file>
@@ -324,7 +338,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +365,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -599,8 +619,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -649,7 +669,6 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="1">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -664,7 +683,6 @@
               </a:r>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-GB" sz="1100" b="0" i="1">
                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
               </a:endParaRPr>
@@ -1996,7 +2014,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2435,43 +2453,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="9" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2482,85 +2503,88 @@
         <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2571,75 +2595,78 @@
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>0.15540000000000001</v>
       </c>
-      <c r="F2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="19">
+      <c r="G2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="19">
         <v>-2</v>
       </c>
-      <c r="H2" s="19">
+      <c r="I2" s="19">
         <v>12</v>
       </c>
-      <c r="I2" s="19">
+      <c r="J2" s="19">
         <v>3</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="5">
         <v>0.15</v>
       </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
       <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
         <v>0.25</v>
       </c>
-      <c r="P2" s="5">
+      <c r="Q2" s="5">
         <v>0.05</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>12</v>
       </c>
-      <c r="S2" s="5">
+      <c r="T2" s="5">
         <v>0.01</v>
       </c>
-      <c r="T2" s="30">
-        <f>(U2-(1-M2)*U2)/(1-M2)</f>
+      <c r="U2" s="30">
+        <f>(V2-(1-N2)*V2)/(1-N2)</f>
         <v>1.4705882352941173E-2</v>
       </c>
-      <c r="U2" s="30">
-        <f>1/Q2</f>
+      <c r="V2" s="30">
+        <f>1/R2</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
-      <c r="Z2" s="2">
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AB2" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -2650,75 +2677,78 @@
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>0.14680000000000001</v>
       </c>
-      <c r="F3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="19">
+      <c r="G3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="19">
         <v>-2</v>
       </c>
-      <c r="H3" s="19">
+      <c r="I3" s="19">
         <v>12</v>
       </c>
-      <c r="I3" s="19">
+      <c r="J3" s="19">
         <v>3</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N3" s="5">
         <v>0.3</v>
       </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
       <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
         <v>0.25</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="5">
         <v>0.05</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>12</v>
       </c>
-      <c r="S3" s="5">
+      <c r="T3" s="5">
         <v>0.01</v>
       </c>
-      <c r="T3" s="30">
-        <f t="shared" ref="T3:T5" si="0">(U3-(1-M3)*U3)/(1-M3)</f>
+      <c r="U3" s="30">
+        <f t="shared" ref="U3:U5" si="0">(V3-(1-N3)*V3)/(1-N3)</f>
         <v>3.5714285714285719E-2</v>
       </c>
-      <c r="U3" s="30">
-        <f t="shared" ref="U3:U5" si="1">1/Q3</f>
+      <c r="V3" s="30">
+        <f t="shared" ref="V3:V5" si="1">1/R3</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="2">
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AB3" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AC3" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2729,67 +2759,70 @@
         <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>0.1153</v>
       </c>
-      <c r="F4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="19">
+      <c r="G4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="19">
         <v>-2</v>
       </c>
-      <c r="H4" s="19">
+      <c r="I4" s="19">
         <v>12</v>
       </c>
-      <c r="I4" s="19">
+      <c r="J4" s="19">
         <v>3</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="M4" s="6">
+      <c r="L4" s="2"/>
+      <c r="N4" s="6">
         <v>0.5</v>
       </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
         <v>12</v>
       </c>
-      <c r="R4" s="6">
+      <c r="S4" s="6">
         <v>1</v>
       </c>
-      <c r="T4" s="30">
+      <c r="U4" s="30">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="U4" s="30">
+      <c r="V4" s="30">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="2">
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AB4" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AC4" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2800,67 +2833,71 @@
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>0.10680000000000001</v>
       </c>
-      <c r="F5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="19">
+      <c r="G5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="19">
         <v>-2</v>
       </c>
-      <c r="H5" s="19">
+      <c r="I5" s="19">
         <v>12</v>
       </c>
-      <c r="I5" s="19">
+      <c r="J5" s="19">
         <v>3</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
+      <c r="L5" s="2"/>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
         <v>12</v>
       </c>
-      <c r="R5" s="6">
+      <c r="S5" s="6">
         <v>0.7</v>
       </c>
-      <c r="T5" s="30">
+      <c r="U5" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U5" s="30">
+      <c r="V5" s="30">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="2">
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AB5" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AC5" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AD5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3082,11 +3119,11 @@
         <v>0</v>
       </c>
       <c r="G7" s="15">
-        <f>(1-H7)*_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$M$2:$M$5)</f>
+        <f>(1-H7)*_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
         <v>0.10374522481551277</v>
       </c>
       <c r="H7" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$H$2:$H$5)*(_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$T$2:$T$5)+_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
         <v>0.30836516789658153</v>
       </c>
       <c r="I7" s="15">
@@ -3288,11 +3325,11 @@
         <v>0</v>
       </c>
       <c r="G14" s="15">
-        <f>(1-H14)*_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$M$2:$M$5)</f>
+        <f>(1-H14)*_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
         <v>0.22810468906746723</v>
       </c>
       <c r="H14" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$H$2:$H$5)*(_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$T$2:$T$5)+_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
         <v>0.23965103644177585</v>
       </c>
       <c r="I14" s="15">
@@ -3494,11 +3531,11 @@
         <v>0</v>
       </c>
       <c r="G21" s="15">
-        <f>(1-H21)*_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$M$2:$M$5)</f>
+        <f>(1-H21)*_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
         <v>0.43233235838169365</v>
       </c>
       <c r="H21" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$H$2:$H$5)*(_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$T$2:$T$5)+_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
         <v>0.1353352832366127</v>
       </c>
       <c r="I21" s="15">
@@ -3700,11 +3737,11 @@
         <v>0</v>
       </c>
       <c r="G28" s="15">
-        <f>(1-H28)*_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$M$2:$M$5)</f>
+        <f>(1-H28)*_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
         <v>0</v>
       </c>
       <c r="H28" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$H$2:$H$5)*(_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$T$2:$T$5)+_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
         <v>0.36787944117144233</v>
       </c>
       <c r="I28" s="15">
@@ -3932,10 +3969,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3989,12 +4026,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>40</v>
@@ -4002,109 +4039,109 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B8" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C8" s="14" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C12" s="14" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>62</v>
@@ -4112,10 +4149,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>62</v>
@@ -4123,10 +4160,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>62</v>
@@ -4134,43 +4171,43 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>62</v>
@@ -4181,73 +4218,73 @@
         <v>74</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    <row r="26" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B26" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>62</v>
@@ -4255,23 +4292,34 @@
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B31" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C31" s="14" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add constant growth LGD model change collateral_index to index add indexed unsecured LGD
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1761419D-063F-4F0D-BB6E-2998D6556D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3A8D43-EA3E-4529-94D0-472096D0C487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37920" yWindow="-4236" windowWidth="30084" windowHeight="12708" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>segment_name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>ead_fees_pct</t>
   </si>
   <si>
-    <t>lgd_collateral_index</t>
-  </si>
-  <si>
     <t>HPI</t>
   </si>
   <si>
@@ -174,12 +171,6 @@
   </si>
   <si>
     <t>The asset correlation parameter Rho.</t>
-  </si>
-  <si>
-    <t>The LGD model to apply. The following values are supported:
-- CONSTANT
-- SECURED
-- UNSECURED</t>
   </si>
   <si>
     <t>The LGD for the CONSTANT LGD model.</t>
@@ -327,6 +318,23 @@
     Typically leads to more macro sensitivity and higher PDs.
 METHOD-2:
     Use the Credit Metrics method where bin widths are fixed and only shifted by the Z-factor.</t>
+  </si>
+  <si>
+    <t>lgd_growth_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The constant growth rate to use for the CONSTANT-GROWTH LGD model. The values is expressed as an effective annual rate. </t>
+  </si>
+  <si>
+    <t>lgd_index</t>
+  </si>
+  <si>
+    <t>The LGD model to apply. The following values are supported:
+- CONSTANT
+- CONSTANT-GROWTH
+- INDEXED
+- SECURED
+- UNSECURED</t>
   </si>
 </sst>
 </file>
@@ -2453,10 +2461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,26 +2481,27 @@
     <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="9" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2500,105 +2509,108 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="AB1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3">
         <v>0.15540000000000001</v>
@@ -2616,71 +2628,71 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="5">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="5">
         <v>0.15</v>
       </c>
-      <c r="O2" s="5">
-        <v>0</v>
-      </c>
       <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
         <v>0.25</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="R2" s="5">
         <v>0.05</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>12</v>
       </c>
-      <c r="T2" s="5">
+      <c r="U2" s="5">
         <v>0.01</v>
       </c>
-      <c r="U2" s="30">
-        <f>(V2-(1-N2)*V2)/(1-N2)</f>
+      <c r="V2" s="30">
+        <f>(W2-(1-O2)*W2)/(1-O2)</f>
         <v>1.4705882352941173E-2</v>
       </c>
-      <c r="V2" s="30">
-        <f>1/R2</f>
+      <c r="W2" s="30">
+        <f>1/S2</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="W2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="5"/>
+      <c r="X2" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
-      <c r="AA2" s="2">
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AC2" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AD2" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3">
         <v>0.14680000000000001</v>
@@ -2698,71 +2710,71 @@
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="5">
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="5">
         <v>0.3</v>
       </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
       <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
         <v>0.25</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="5">
         <v>0.05</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>12</v>
       </c>
-      <c r="T3" s="5">
+      <c r="U3" s="5">
         <v>0.01</v>
       </c>
-      <c r="U3" s="30">
-        <f t="shared" ref="U3:U5" si="0">(V3-(1-N3)*V3)/(1-N3)</f>
+      <c r="V3" s="30">
+        <f t="shared" ref="V3:V5" si="0">(W3-(1-O3)*W3)/(1-O3)</f>
         <v>3.5714285714285719E-2</v>
       </c>
-      <c r="V3" s="30">
-        <f t="shared" ref="V3:V5" si="1">1/R3</f>
+      <c r="W3" s="30">
+        <f t="shared" ref="W3:W5" si="1">1/S3</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="W3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" s="5"/>
+      <c r="X3" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="2">
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AC3" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AD3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AD3" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="4">
         <v>0.1153</v>
@@ -2780,63 +2792,64 @@
         <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="N4" s="6">
+      <c r="M4" s="2"/>
+      <c r="O4" s="6">
         <v>0.5</v>
       </c>
-      <c r="O4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2">
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
         <v>12</v>
       </c>
-      <c r="S4" s="6">
+      <c r="T4" s="6">
         <v>1</v>
       </c>
-      <c r="U4" s="30">
+      <c r="V4" s="30">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="V4" s="30">
+      <c r="W4" s="30">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="X4" s="5"/>
+      <c r="X4" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="2">
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AC4" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AD4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AD4" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4">
         <v>0.10680000000000001</v>
@@ -2854,46 +2867,47 @@
         <v>3</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2">
+      <c r="M5" s="2"/>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
         <v>12</v>
       </c>
-      <c r="S5" s="6">
+      <c r="T5" s="6">
         <v>0.7</v>
       </c>
-      <c r="U5" s="30">
+      <c r="V5" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V5" s="30">
+      <c r="W5" s="30">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="W5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="X5" s="5"/>
+      <c r="X5" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="2">
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="2">
         <v>0.5</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>1E-3</v>
       </c>
       <c r="AC5" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AD5" s="2" t="s">
-        <v>17</v>
+      <c r="AD5" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2933,7 +2947,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="17">
         <v>1</v>
@@ -2948,10 +2962,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2959,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="24">
         <v>1</v>
@@ -3104,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="15">
         <v>0</v>
@@ -3119,11 +3133,11 @@
         <v>0</v>
       </c>
       <c r="G7" s="15">
-        <f>(1-H7)*_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
+        <f>(1-H7)*_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$O$2:$O$5)</f>
         <v>0.10374522481551277</v>
       </c>
       <c r="H7" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)+_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$W$2:$W$5)))</f>
         <v>0.30836516789658153</v>
       </c>
       <c r="I7" s="15">
@@ -3136,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="28">
         <v>0</v>
@@ -3165,7 +3179,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="24">
         <v>1</v>
@@ -3310,7 +3324,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="15">
         <v>0</v>
@@ -3325,11 +3339,11 @@
         <v>0</v>
       </c>
       <c r="G14" s="15">
-        <f>(1-H14)*_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
+        <f>(1-H14)*_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$O$2:$O$5)</f>
         <v>0.22810468906746723</v>
       </c>
       <c r="H14" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)+_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$W$2:$W$5)))</f>
         <v>0.23965103644177585</v>
       </c>
       <c r="I14" s="15">
@@ -3342,7 +3356,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" s="28">
         <v>0</v>
@@ -3371,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="24">
         <v>1</v>
@@ -3516,7 +3530,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="15">
         <v>0</v>
@@ -3531,11 +3545,11 @@
         <v>0</v>
       </c>
       <c r="G21" s="15">
-        <f>(1-H21)*_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
+        <f>(1-H21)*_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$O$2:$O$5)</f>
         <v>0.43233235838169365</v>
       </c>
       <c r="H21" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)+_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$W$2:$W$5)))</f>
         <v>0.1353352832366127</v>
       </c>
       <c r="I21" s="15">
@@ -3548,7 +3562,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="28">
         <v>0</v>
@@ -3577,7 +3591,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="24">
         <v>1</v>
@@ -3722,7 +3736,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="15">
         <v>0</v>
@@ -3737,11 +3751,11 @@
         <v>0</v>
       </c>
       <c r="G28" s="15">
-        <f>(1-H28)*_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$N$2:$N$5)</f>
+        <f>(1-H28)*_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$O$2:$O$5)</f>
         <v>0</v>
       </c>
       <c r="H28" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$U$2:$U$5)+_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)))</f>
+        <f>EXP(-_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$I$2:$I$5)*(_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$V$2:$V$5)+_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$5,ASSUMPTIONS!$W$2:$W$5)))</f>
         <v>0.36787944117144233</v>
       </c>
       <c r="I28" s="15">
@@ -3754,7 +3768,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="28">
         <v>0</v>
@@ -3802,10 +3816,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="17">
         <v>1</v>
@@ -3820,10 +3834,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3969,10 +3983,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,13 +3998,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3998,10 +4012,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4009,43 +4023,43 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4053,274 +4067,285 @@
         <v>2</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="B22" s="13" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>34</v>
-      </c>
       <c r="B27" s="13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>13</v>
-      </c>
       <c r="B29" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B31" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>40</v>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add default penalties to amortising EAD
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\geyerbisschoff\pythonprojects\z-model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52839319-1780-4A07-9703-07E0B2EF851B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A68958-DB73-4BE8-A5F6-9A6D8D3AA5A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="99">
   <si>
     <t>segment_name</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>Segment 5</t>
+  </si>
+  <si>
+    <t>ead_default_penalty_pct</t>
+  </si>
+  <si>
+    <t>ead_default_penalty_amt</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -536,6 +542,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2485,10 +2492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2523,10 +2530,12 @@
     <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2618,10 +2627,16 @@
         <v>11</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -2688,11 +2703,13 @@
       <c r="AA2" s="5"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -2742,11 +2759,11 @@
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="30">
-        <f t="shared" ref="V3:V5" si="0">(W3-(1-O3)*W3)/(1-O3)</f>
+        <f t="shared" ref="V3:V4" si="0">(W3-(1-O3)*W3)/(1-O3)</f>
         <v>0.19444444444444439</v>
       </c>
       <c r="W3" s="30">
-        <f t="shared" ref="W3:W5" si="1">1/S3</f>
+        <f t="shared" ref="W3:W4" si="1">1/S3</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="X3" s="5" t="s">
@@ -2764,11 +2781,17 @@
       <c r="AD3" s="3">
         <v>1E-3</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AE3" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="AF3" s="31">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -2840,11 +2863,13 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="2" t="s">
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
@@ -2923,11 +2948,13 @@
       <c r="AB5" s="2"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="2" t="s">
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>96</v>
       </c>
@@ -2996,7 +3023,9 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="2" t="s">
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3011,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
move PWO calculations from Excel template to the code.
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A68958-DB73-4BE8-A5F6-9A6D8D3AA5A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669C8767-71D4-4A47-9E3F-639297336C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="DICTIONARY" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TRANSITION_MATRIX!$A$1:$A$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TRANSITION_MATRIX!$A$1:$A$14</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
   <si>
     <t>segment_name</t>
   </si>
@@ -236,9 +236,6 @@
     <t>pd_frequency</t>
   </si>
   <si>
-    <t>pd_default_state</t>
-  </si>
-  <si>
     <t>pd_time_in_watchlist</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
   </si>
   <si>
     <t>lgd_mu_c</t>
-  </si>
-  <si>
-    <t>lgd_mu_w</t>
   </si>
   <si>
     <t>&lt;bool&gt;</t>
@@ -265,9 +259,6 @@
     PiT = N(TtC -  Z * (Rho ** 0.5) / (1 - Rho) ** 0.5)</t>
   </si>
   <si>
-    <t>The default state column index in the Transition Matrix</t>
-  </si>
-  <si>
     <t>The frequency of the transition matrix</t>
   </si>
   <si>
@@ -366,15 +357,20 @@
   <si>
     <t>ead_default_penalty_amt</t>
   </si>
+  <si>
+    <t>pd_cure_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The column index in the Transition Matrix to which defaults cure. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -440,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -468,21 +464,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -536,12 +523,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -647,19 +628,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>565785</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>567690</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -673,8 +654,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7566660" y="232410"/>
-              <a:ext cx="5191125" cy="2678430"/>
+              <a:off x="6819900" y="232410"/>
+              <a:ext cx="5193030" cy="3097530"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2053,7 +2034,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2067,8 +2048,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7566660" y="232410"/>
-              <a:ext cx="5191125" cy="2678430"/>
+              <a:off x="6819900" y="232410"/>
+              <a:ext cx="5193030" cy="3097530"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2102,7 +2083,6 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="1">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2117,7 +2097,6 @@
               </a:r>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-GB" sz="1100" b="0" i="1">
                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
               </a:endParaRPr>
@@ -2492,10 +2471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF17" sqref="AF17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,21 +2500,19 @@
     <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" customWidth="1"/>
-    <col min="24" max="24" width="14.5703125" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" customWidth="1"/>
+    <col min="23" max="23" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.140625" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2546,7 +2523,7 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -2555,16 +2532,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>21</v>
@@ -2573,10 +2550,10 @@
         <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>3</v>
@@ -2600,45 +2577,39 @@
         <v>9</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2647,7 +2618,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
@@ -2659,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="19">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="19">
         <v>12</v>
@@ -2668,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L2" s="5">
         <v>0.5</v>
@@ -2685,33 +2656,25 @@
         <v>12</v>
       </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="30">
-        <f>(W2-(1-O2)*W2)/(1-O2)</f>
-        <v>0.19444444444444439</v>
-      </c>
-      <c r="W2" s="30">
-        <f>1/S2</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
+      <c r="V2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="5">
+        <v>1</v>
+      </c>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -2720,7 +2683,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>17</v>
@@ -2732,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="19">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="19">
         <v>12</v>
@@ -2741,7 +2704,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M3" s="5">
         <v>0.05</v>
@@ -2758,42 +2721,34 @@
         <v>12</v>
       </c>
       <c r="U3" s="5"/>
-      <c r="V3" s="30">
-        <f t="shared" ref="V3:V4" si="0">(W3-(1-O3)*W3)/(1-O3)</f>
-        <v>0.19444444444444439</v>
-      </c>
-      <c r="W3" s="30">
-        <f t="shared" ref="W3:W4" si="1">1/S3</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="X3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="2">
+      <c r="Z3" s="2">
         <v>0.5</v>
       </c>
+      <c r="AA3" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>1E-3</v>
+      </c>
       <c r="AC3" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="AE3" s="3">
         <v>0.02</v>
       </c>
-      <c r="AF3" s="31">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AD3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -2802,7 +2757,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
@@ -2814,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="19">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I4" s="19">
         <v>12</v>
@@ -2823,14 +2778,14 @@
         <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L4" s="5">
         <v>0.5</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O4" s="6">
         <v>0.7</v>
@@ -2842,36 +2797,28 @@
         <v>12</v>
       </c>
       <c r="T4" s="6"/>
-      <c r="V4" s="30">
-        <f t="shared" si="0"/>
-        <v>0.19444444444444439</v>
-      </c>
-      <c r="W4" s="30">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="V4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="W4" s="5"/>
       <c r="X4" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -2880,7 +2827,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
@@ -2892,7 +2839,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="19">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="19">
         <v>12</v>
@@ -2927,36 +2874,28 @@
       <c r="U5" s="5">
         <v>0.01</v>
       </c>
-      <c r="V5" s="30">
-        <f>(W5-(1-O5)*W5)/(1-O5)</f>
-        <v>0.19444444444444439</v>
-      </c>
-      <c r="W5" s="30">
-        <f>1/S5</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="V5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="W5" s="5"/>
       <c r="X5" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -2965,7 +2904,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
@@ -2977,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="19">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I6" s="19">
         <v>12</v>
@@ -3002,30 +2941,22 @@
       <c r="T6" s="6">
         <v>1</v>
       </c>
-      <c r="V6" s="30">
-        <f t="shared" ref="V6" si="2">(W6-(1-O6)*W6)/(1-O6)</f>
-        <v>0.19444444444444439</v>
-      </c>
-      <c r="W6" s="30">
-        <f t="shared" ref="W6" si="3">1/S6</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="V6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="W6" s="5"/>
       <c r="X6" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3038,10 +2969,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3053,12 +2984,12 @@
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" customWidth="1"/>
-    <col min="12" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -3083,11 +3014,8 @@
       <c r="H1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -3112,11 +3040,8 @@
       <c r="H2" s="26">
         <v>0</v>
       </c>
-      <c r="I2" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -3141,11 +3066,8 @@
       <c r="H3" s="15">
         <v>0.01</v>
       </c>
-      <c r="I3" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -3170,11 +3092,8 @@
       <c r="H4" s="15">
         <v>0.02</v>
       </c>
-      <c r="I4" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>1</v>
       </c>
@@ -3199,11 +3118,8 @@
       <c r="H5" s="15">
         <v>0.05</v>
       </c>
-      <c r="I5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>1</v>
       </c>
@@ -3228,11 +3144,8 @@
       <c r="H6" s="15">
         <v>0.1</v>
       </c>
-      <c r="I6" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>1</v>
       </c>
@@ -3252,873 +3165,638 @@
         <v>0</v>
       </c>
       <c r="G7" s="15">
-        <f>(1-H7)*_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$O$2:$O$10)</f>
-        <v>0.67502820465692326</v>
+        <v>0</v>
       </c>
       <c r="H7" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$I$2:$I$10)*(_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$V$2:$V$10)+_xlfn.XLOOKUP(A7,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$W$2:$W$10)))</f>
-        <v>3.5673993347252408E-2</v>
-      </c>
-      <c r="I7" s="15">
-        <f>1-SUM(G7:H7)</f>
-        <v>0.28929780199582433</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
-        <v>1</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="28">
-        <v>0</v>
-      </c>
-      <c r="D8" s="28">
-        <v>0</v>
-      </c>
-      <c r="E8" s="28">
-        <v>0</v>
-      </c>
-      <c r="F8" s="28">
-        <v>0</v>
-      </c>
-      <c r="G8" s="28">
-        <v>0</v>
-      </c>
-      <c r="H8" s="28">
-        <v>0</v>
-      </c>
-      <c r="I8" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="24">
-        <v>1</v>
-      </c>
-      <c r="D9" s="25">
-        <v>0</v>
-      </c>
-      <c r="E9" s="26">
-        <v>0</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0</v>
-      </c>
-      <c r="H9" s="26">
-        <v>0</v>
-      </c>
-      <c r="I9" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="25">
+        <v>0</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0</v>
+      </c>
+      <c r="H8" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.67768484848484856</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.20243434343434344</v>
+      </c>
+      <c r="F9" s="15">
+        <v>6.830303030303031E-2</v>
+      </c>
+      <c r="G9" s="15">
+        <v>3.1577777777777774E-2</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>2</v>
       </c>
       <c r="B10" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="21">
         <v>0.01</v>
       </c>
-      <c r="D10" s="20">
-        <v>0.67768484848484856</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0.20243434343434344</v>
+      <c r="D10" s="15">
+        <v>0.33851020408163268</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0.40185714285714286</v>
       </c>
       <c r="F10" s="15">
-        <v>6.830303030303031E-2</v>
+        <v>0.15698163265306123</v>
       </c>
       <c r="G10" s="15">
-        <v>3.1577777777777774E-2</v>
+        <v>7.2651020408163278E-2</v>
       </c>
       <c r="H10" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>2</v>
       </c>
       <c r="B11" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="21">
         <v>0.01</v>
       </c>
       <c r="D11" s="15">
-        <v>0.33851020408163268</v>
-      </c>
-      <c r="E11" s="20">
-        <v>0.40185714285714286</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0.15698163265306123</v>
+        <v>9.2713684210526323E-2</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.18780210526315788</v>
+      </c>
+      <c r="F11" s="20">
+        <v>0.41033473684210525</v>
       </c>
       <c r="G11" s="15">
-        <v>7.2651020408163278E-2</v>
+        <v>0.24914947368421053</v>
       </c>
       <c r="H11" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>2</v>
       </c>
       <c r="B12" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="21">
         <v>0.01</v>
       </c>
       <c r="D12" s="15">
-        <v>9.2713684210526323E-2</v>
+        <v>2.857888888888889E-2</v>
       </c>
       <c r="E12" s="15">
-        <v>0.18780210526315788</v>
-      </c>
-      <c r="F12" s="20">
-        <v>0.41033473684210525</v>
-      </c>
-      <c r="G12" s="15">
-        <v>0.24914947368421053</v>
+        <v>5.7850000000000006E-2</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0.18670222222222221</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0.61686888888888891</v>
       </c>
       <c r="H12" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>2</v>
       </c>
-      <c r="B13" s="16">
-        <v>4</v>
-      </c>
-      <c r="C13" s="21">
+      <c r="B13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
+        <v>3</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="25">
+        <v>0</v>
+      </c>
+      <c r="E14" s="26">
+        <v>0</v>
+      </c>
+      <c r="F14" s="26">
+        <v>0</v>
+      </c>
+      <c r="G14" s="26">
+        <v>0</v>
+      </c>
+      <c r="H14" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>3</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21">
         <v>0.01</v>
       </c>
-      <c r="D13" s="15">
-        <v>2.857888888888889E-2</v>
-      </c>
-      <c r="E13" s="15">
-        <v>5.7850000000000006E-2</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0.18670222222222221</v>
-      </c>
-      <c r="G13" s="20">
-        <v>0.61686888888888891</v>
-      </c>
-      <c r="H13" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="D15" s="20">
+        <v>0.67768484848484856</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.20243434343434344</v>
+      </c>
+      <c r="F15" s="15">
+        <v>6.830303030303031E-2</v>
+      </c>
+      <c r="G15" s="15">
+        <v>3.1577777777777774E-2</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>3</v>
+      </c>
+      <c r="B16" s="16">
         <v>2</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="15">
-        <v>0</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0</v>
-      </c>
-      <c r="F14" s="15">
-        <v>0</v>
-      </c>
-      <c r="G14" s="15">
-        <f>(1-H14)*_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$O$2:$O$10)</f>
-        <v>0.67502820465692326</v>
-      </c>
-      <c r="H14" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$I$2:$I$10)*(_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$V$2:$V$10)+_xlfn.XLOOKUP(A14,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$W$2:$W$10)))</f>
-        <v>3.5673993347252408E-2</v>
-      </c>
-      <c r="I14" s="15">
-        <f>1-SUM(G14:H14)</f>
-        <v>0.28929780199582433</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
-        <v>2</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="28">
-        <v>0</v>
-      </c>
-      <c r="D15" s="28">
-        <v>0</v>
-      </c>
-      <c r="E15" s="28">
-        <v>0</v>
-      </c>
-      <c r="F15" s="28">
-        <v>0</v>
-      </c>
-      <c r="G15" s="28">
-        <v>0</v>
-      </c>
-      <c r="H15" s="28">
-        <v>0</v>
-      </c>
-      <c r="I15" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
-        <v>3</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="24">
-        <v>1</v>
-      </c>
-      <c r="D16" s="25">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26">
-        <v>0</v>
-      </c>
-      <c r="I16" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.33851020408163268</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0.40185714285714286</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0.15698163265306123</v>
+      </c>
+      <c r="G16" s="15">
+        <v>7.2651020408163278E-2</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>3</v>
       </c>
       <c r="B17" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="21">
         <v>0.01</v>
       </c>
-      <c r="D17" s="20">
-        <v>0.67768484848484856</v>
+      <c r="D17" s="15">
+        <v>9.2713684210526323E-2</v>
       </c>
       <c r="E17" s="15">
-        <v>0.20243434343434344</v>
-      </c>
-      <c r="F17" s="15">
-        <v>6.830303030303031E-2</v>
+        <v>0.18780210526315788</v>
+      </c>
+      <c r="F17" s="20">
+        <v>0.41033473684210525</v>
       </c>
       <c r="G17" s="15">
-        <v>3.1577777777777774E-2</v>
+        <v>0.24914947368421053</v>
       </c>
       <c r="H17" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="I17" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>3</v>
       </c>
       <c r="B18" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18" s="21">
         <v>0.01</v>
       </c>
       <c r="D18" s="15">
-        <v>0.33851020408163268</v>
-      </c>
-      <c r="E18" s="20">
-        <v>0.40185714285714286</v>
+        <v>2.857888888888889E-2</v>
+      </c>
+      <c r="E18" s="15">
+        <v>5.7850000000000006E-2</v>
       </c>
       <c r="F18" s="15">
-        <v>0.15698163265306123</v>
-      </c>
-      <c r="G18" s="15">
-        <v>7.2651020408163278E-2</v>
+        <v>0.18670222222222221</v>
+      </c>
+      <c r="G18" s="20">
+        <v>0.61686888888888891</v>
       </c>
       <c r="H18" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="I18" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>3</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
+        <v>4</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="24">
+        <v>1</v>
+      </c>
+      <c r="D20" s="25">
+        <v>0</v>
+      </c>
+      <c r="E20" s="26">
+        <v>0</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0</v>
+      </c>
+      <c r="H20" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>4</v>
+      </c>
+      <c r="B21" s="16">
+        <v>1</v>
+      </c>
+      <c r="C21" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.67768484848484856</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.20243434343434344</v>
+      </c>
+      <c r="F21" s="15">
+        <v>6.830303030303031E-2</v>
+      </c>
+      <c r="G21" s="15">
+        <v>3.1577777777777774E-2</v>
+      </c>
+      <c r="H21" s="15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>4</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2</v>
+      </c>
+      <c r="C22" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D22" s="15">
+        <v>0.33851020408163268</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0.40185714285714286</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0.15698163265306123</v>
+      </c>
+      <c r="G22" s="15">
+        <v>7.2651020408163278E-2</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>4</v>
+      </c>
+      <c r="B23" s="16">
         <v>3</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C23" s="21">
         <v>0.01</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D23" s="15">
         <v>9.2713684210526323E-2</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E23" s="15">
         <v>0.18780210526315788</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F23" s="20">
         <v>0.41033473684210525</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G23" s="15">
         <v>0.24914947368421053</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H23" s="15">
         <v>0.05</v>
       </c>
-      <c r="I19" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
-        <v>3</v>
-      </c>
-      <c r="B20" s="16">
-        <v>4</v>
-      </c>
-      <c r="C20" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="D20" s="15">
-        <v>2.857888888888889E-2</v>
-      </c>
-      <c r="E20" s="15">
-        <v>5.7850000000000006E-2</v>
-      </c>
-      <c r="F20" s="15">
-        <v>0.18670222222222221</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0.61686888888888891</v>
-      </c>
-      <c r="H20" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="I20" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
-        <v>3</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="15">
-        <v>0</v>
-      </c>
-      <c r="D21" s="15">
-        <v>0</v>
-      </c>
-      <c r="E21" s="15">
-        <v>0</v>
-      </c>
-      <c r="F21" s="15">
-        <v>0</v>
-      </c>
-      <c r="G21" s="15">
-        <f>(1-H21)*_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$O$2:$O$10)</f>
-        <v>0.67502820465692326</v>
-      </c>
-      <c r="H21" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$I$2:$I$10)*(_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$V$2:$V$10)+_xlfn.XLOOKUP(A21,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$W$2:$W$10)))</f>
-        <v>3.5673993347252408E-2</v>
-      </c>
-      <c r="I21" s="15">
-        <f>1-SUM(G21:H21)</f>
-        <v>0.28929780199582433</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
-        <v>3</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="28">
-        <v>0</v>
-      </c>
-      <c r="D22" s="28">
-        <v>0</v>
-      </c>
-      <c r="E22" s="28">
-        <v>0</v>
-      </c>
-      <c r="F22" s="28">
-        <v>0</v>
-      </c>
-      <c r="G22" s="28">
-        <v>0</v>
-      </c>
-      <c r="H22" s="28">
-        <v>0</v>
-      </c>
-      <c r="I22" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
-        <v>4</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="24">
-        <v>1</v>
-      </c>
-      <c r="D23" s="25">
-        <v>0</v>
-      </c>
-      <c r="E23" s="26">
-        <v>0</v>
-      </c>
-      <c r="F23" s="26">
-        <v>0</v>
-      </c>
-      <c r="G23" s="26">
-        <v>0</v>
-      </c>
-      <c r="H23" s="26">
-        <v>0</v>
-      </c>
-      <c r="I23" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>4</v>
       </c>
       <c r="B24" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" s="21">
         <v>0.01</v>
       </c>
-      <c r="D24" s="20">
-        <v>0.67768484848484856</v>
+      <c r="D24" s="15">
+        <v>2.857888888888889E-2</v>
       </c>
       <c r="E24" s="15">
-        <v>0.20243434343434344</v>
+        <v>5.7850000000000006E-2</v>
       </c>
       <c r="F24" s="15">
-        <v>6.830303030303031E-2</v>
-      </c>
-      <c r="G24" s="15">
-        <v>3.1577777777777774E-2</v>
+        <v>0.18670222222222221</v>
+      </c>
+      <c r="G24" s="20">
+        <v>0.61686888888888891</v>
       </c>
       <c r="H24" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="I24" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>4</v>
       </c>
-      <c r="B25" s="16">
-        <v>2</v>
-      </c>
-      <c r="C25" s="21">
-        <v>0.01</v>
+      <c r="B25" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="15">
+        <v>0</v>
       </c>
       <c r="D25" s="15">
-        <v>0.33851020408163268</v>
-      </c>
-      <c r="E25" s="20">
-        <v>0.40185714285714286</v>
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
+        <v>0</v>
       </c>
       <c r="F25" s="15">
-        <v>0.15698163265306123</v>
+        <v>0</v>
       </c>
       <c r="G25" s="15">
-        <v>7.2651020408163278E-2</v>
-      </c>
-      <c r="H25" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="I25" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
-        <v>4</v>
-      </c>
-      <c r="B26" s="16">
-        <v>3</v>
-      </c>
-      <c r="C26" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="D26" s="15">
-        <v>9.2713684210526323E-2</v>
-      </c>
-      <c r="E26" s="15">
-        <v>0.18780210526315788</v>
-      </c>
-      <c r="F26" s="20">
-        <v>0.41033473684210525</v>
-      </c>
-      <c r="G26" s="15">
-        <v>0.24914947368421053</v>
-      </c>
-      <c r="H26" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="I26" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>5</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="24">
+        <v>1</v>
+      </c>
+      <c r="D26" s="25">
+        <v>0</v>
+      </c>
+      <c r="E26" s="26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C27" s="21">
         <v>0.01</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="20">
+        <v>0.67768484848484856</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0.20243434343434344</v>
+      </c>
+      <c r="F27" s="15">
+        <v>6.830303030303031E-2</v>
+      </c>
+      <c r="G27" s="15">
+        <v>3.1577777777777774E-2</v>
+      </c>
+      <c r="H27" s="15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>5</v>
+      </c>
+      <c r="B28" s="16">
+        <v>2</v>
+      </c>
+      <c r="C28" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D28" s="15">
+        <v>0.33851020408163268</v>
+      </c>
+      <c r="E28" s="20">
+        <v>0.40185714285714286</v>
+      </c>
+      <c r="F28" s="15">
+        <v>0.15698163265306123</v>
+      </c>
+      <c r="G28" s="15">
+        <v>7.2651020408163278E-2</v>
+      </c>
+      <c r="H28" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>5</v>
+      </c>
+      <c r="B29" s="16">
+        <v>3</v>
+      </c>
+      <c r="C29" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D29" s="15">
+        <v>9.2713684210526323E-2</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.18780210526315788</v>
+      </c>
+      <c r="F29" s="20">
+        <v>0.41033473684210525</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0.24914947368421053</v>
+      </c>
+      <c r="H29" s="15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>5</v>
+      </c>
+      <c r="B30" s="16">
+        <v>4</v>
+      </c>
+      <c r="C30" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="D30" s="15">
         <v>2.857888888888889E-2</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E30" s="15">
         <v>5.7850000000000006E-2</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F30" s="15">
         <v>0.18670222222222221</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G30" s="20">
         <v>0.61686888888888891</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H30" s="15">
         <v>0.1</v>
       </c>
-      <c r="I27" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
-        <v>4</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="15">
-        <v>0</v>
-      </c>
-      <c r="D28" s="15">
-        <v>0</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0</v>
-      </c>
-      <c r="F28" s="15">
-        <v>0</v>
-      </c>
-      <c r="G28" s="15">
-        <f>(1-H28)*_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$O$2:$O$10)</f>
-        <v>0.67502820465692326</v>
-      </c>
-      <c r="H28" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$I$2:$I$10)*(_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$V$2:$V$10)+_xlfn.XLOOKUP(A28,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$W$2:$W$10)))</f>
-        <v>3.5673993347252408E-2</v>
-      </c>
-      <c r="I28" s="15">
-        <f>1-SUM(G28:H28)</f>
-        <v>0.28929780199582433</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
-        <v>4</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="28">
-        <v>0</v>
-      </c>
-      <c r="D29" s="28">
-        <v>0</v>
-      </c>
-      <c r="E29" s="28">
-        <v>0</v>
-      </c>
-      <c r="F29" s="28">
-        <v>0</v>
-      </c>
-      <c r="G29" s="28">
-        <v>0</v>
-      </c>
-      <c r="H29" s="28">
-        <v>0</v>
-      </c>
-      <c r="I29" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
-        <v>5</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="24">
-        <v>1</v>
-      </c>
-      <c r="D30" s="25">
-        <v>0</v>
-      </c>
-      <c r="E30" s="26">
-        <v>0</v>
-      </c>
-      <c r="F30" s="26">
-        <v>0</v>
-      </c>
-      <c r="G30" s="26">
-        <v>0</v>
-      </c>
-      <c r="H30" s="26">
-        <v>0</v>
-      </c>
-      <c r="I30" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>5</v>
       </c>
-      <c r="B31" s="16">
-        <v>1</v>
-      </c>
-      <c r="C31" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="D31" s="20">
-        <v>0.67768484848484856</v>
+      <c r="B31" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="15">
+        <v>0</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0</v>
       </c>
       <c r="E31" s="15">
-        <v>0.20243434343434344</v>
+        <v>0</v>
       </c>
       <c r="F31" s="15">
-        <v>6.830303030303031E-2</v>
+        <v>0</v>
       </c>
       <c r="G31" s="15">
-        <v>3.1577777777777774E-2</v>
-      </c>
-      <c r="H31" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="I31" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="16">
-        <v>5</v>
-      </c>
-      <c r="B32" s="16">
-        <v>2</v>
-      </c>
-      <c r="C32" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="D32" s="15">
-        <v>0.33851020408163268</v>
-      </c>
-      <c r="E32" s="20">
-        <v>0.40185714285714286</v>
-      </c>
-      <c r="F32" s="15">
-        <v>0.15698163265306123</v>
-      </c>
-      <c r="G32" s="15">
-        <v>7.2651020408163278E-2</v>
-      </c>
-      <c r="H32" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="I32" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>5</v>
-      </c>
-      <c r="B33" s="16">
-        <v>3</v>
-      </c>
-      <c r="C33" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="D33" s="15">
-        <v>9.2713684210526323E-2</v>
-      </c>
-      <c r="E33" s="15">
-        <v>0.18780210526315788</v>
-      </c>
-      <c r="F33" s="20">
-        <v>0.41033473684210525</v>
-      </c>
-      <c r="G33" s="15">
-        <v>0.24914947368421053</v>
-      </c>
-      <c r="H33" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="I33" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="16">
-        <v>5</v>
-      </c>
-      <c r="B34" s="16">
-        <v>4</v>
-      </c>
-      <c r="C34" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="D34" s="15">
-        <v>2.857888888888889E-2</v>
-      </c>
-      <c r="E34" s="15">
-        <v>5.7850000000000006E-2</v>
-      </c>
-      <c r="F34" s="15">
-        <v>0.18670222222222221</v>
-      </c>
-      <c r="G34" s="20">
-        <v>0.61686888888888891</v>
-      </c>
-      <c r="H34" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="I34" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="16">
-        <v>5</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="15">
-        <v>0</v>
-      </c>
-      <c r="D35" s="15">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="15">
-        <v>0</v>
-      </c>
-      <c r="G35" s="15">
-        <f>(1-H35)*_xlfn.XLOOKUP(A35,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$O$2:$O$10)</f>
-        <v>0.67502820465692326</v>
-      </c>
-      <c r="H35" s="20">
-        <f>EXP(-_xlfn.XLOOKUP(A35,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$I$2:$I$10)*(_xlfn.XLOOKUP(A35,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$V$2:$V$10)+_xlfn.XLOOKUP(A35,ASSUMPTIONS!$B$2:$B$10,ASSUMPTIONS!$W$2:$W$10)))</f>
-        <v>3.5673993347252408E-2</v>
-      </c>
-      <c r="I35" s="15">
-        <f>1-SUM(G35:H35)</f>
-        <v>0.28929780199582433</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
-        <v>5</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="28">
-        <v>0</v>
-      </c>
-      <c r="D36" s="28">
-        <v>0</v>
-      </c>
-      <c r="E36" s="28">
-        <v>0</v>
-      </c>
-      <c r="F36" s="28">
-        <v>0</v>
-      </c>
-      <c r="G36" s="28">
-        <v>0</v>
-      </c>
-      <c r="H36" s="28">
-        <v>0</v>
-      </c>
-      <c r="I36" s="29">
+        <v>0</v>
+      </c>
+      <c r="H31" s="20">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A16" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:A14" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4130,7 +3808,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4310,8 +3988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4359,7 +4037,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>35</v>
@@ -4367,10 +4045,10 @@
     </row>
     <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>35</v>
@@ -4400,21 +4078,21 @@
     </row>
     <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>37</v>
@@ -4425,7 +4103,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>37</v>
@@ -4433,10 +4111,10 @@
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>37</v>
@@ -4447,7 +4125,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>35</v>
@@ -4466,10 +4144,10 @@
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>56</v>
@@ -4477,7 +4155,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>41</v>
@@ -4565,10 +4243,10 @@
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>56</v>
@@ -4576,10 +4254,10 @@
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>56</v>
@@ -4612,7 +4290,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
fix ead for CCF methods when outstanding balance is zero, but off-balance sheet exposure is greater than zero
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669C8767-71D4-4A47-9E3F-639297336C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610D759-8C45-4DB7-B3C3-A52B6DEED63F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40452" yWindow="-6528" windowWidth="40560" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -639,8 +639,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2034,7 +2034,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2473,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,12 +2715,18 @@
       <c r="P3" s="5">
         <v>0</v>
       </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
+      <c r="Q3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.05</v>
+      </c>
       <c r="S3" s="2">
         <v>12</v>
       </c>
-      <c r="U3" s="5"/>
+      <c r="U3" s="5">
+        <v>0.01</v>
+      </c>
       <c r="V3" s="5" t="s">
         <v>25</v>
       </c>
@@ -2971,7 +2977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
make changes for climate risk modelling: - add climate risk templates - update data in other templates to consider climate risk - add climate risk LGD - add ability to do static, business plan and dynamic forecasts - save expanded results as parquet file rather than csv - update pandas dependency - update pytests
</commit_message>
<xml_diff>
--- a/data/ASSUMPTIONS.xlsx
+++ b/data/ASSUMPTIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610D759-8C45-4DB7-B3C3-A52B6DEED63F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A3A591-A66F-4E0A-81B7-EA81C0EED3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40452" yWindow="-6528" windowWidth="40560" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSUMPTIONS" sheetId="2" r:id="rId1"/>
@@ -2473,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,8 +2977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>